<commit_message>
Benchmark on logs table
</commit_message>
<xml_diff>
--- a/EFcore30Benchmark/EFBenchmark_Result.xlsx
+++ b/EFcore30Benchmark/EFBenchmark_Result.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
   <si>
     <t>Spire.XLS for .NET</t>
   </si>
@@ -102,6 +102,33 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>964</t>
+  </si>
+  <si>
+    <t>956</t>
+  </si>
+  <si>
+    <t>954</t>
+  </si>
+  <si>
+    <t>934</t>
+  </si>
+  <si>
+    <t>938</t>
+  </si>
+  <si>
+    <t>952</t>
+  </si>
+  <si>
+    <t>962</t>
+  </si>
+  <si>
+    <t>959</t>
+  </si>
+  <si>
+    <t>930</t>
   </si>
 </sst>
 </file>
@@ -563,7 +590,7 @@
       </bottom>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -587,6 +614,34 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment/>
     </xf>
@@ -736,49 +791,49 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="40% - Accent1" xfId="20"/>
-    <cellStyle name="Check Cell" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Note" xfId="23"/>
-    <cellStyle name="Hyperlink" xfId="24"/>
-    <cellStyle name="60% - Accent4" xfId="25"/>
-    <cellStyle name="Followed Hyperlink" xfId="26"/>
-    <cellStyle name="40% - Accent3" xfId="27"/>
-    <cellStyle name="Warning Text" xfId="28"/>
-    <cellStyle name="40% - Accent2" xfId="29"/>
-    <cellStyle name="Title" xfId="30"/>
-    <cellStyle name="CExplanatory Text" xfId="31"/>
-    <cellStyle name="Heading 1" xfId="32"/>
-    <cellStyle name="Heading 3" xfId="33"/>
-    <cellStyle name="Heading 4" xfId="34"/>
-    <cellStyle name="Input" xfId="35"/>
-    <cellStyle name="60% - Accent3" xfId="36"/>
-    <cellStyle name="Good" xfId="37"/>
-    <cellStyle name="Output" xfId="38"/>
-    <cellStyle name="20% - Accent1" xfId="39"/>
-    <cellStyle name="Calculation" xfId="40"/>
-    <cellStyle name="Linked Cell" xfId="41"/>
-    <cellStyle name="Total" xfId="42"/>
-    <cellStyle name="Bad" xfId="43"/>
-    <cellStyle name="Neutral" xfId="44"/>
-    <cellStyle name="Accent1" xfId="45"/>
-    <cellStyle name="20% - Accent5" xfId="46"/>
-    <cellStyle name="60% - Accent1" xfId="47"/>
-    <cellStyle name="Accent2" xfId="48"/>
-    <cellStyle name="20% - Accent2" xfId="49"/>
-    <cellStyle name="20% - Accent6" xfId="50"/>
-    <cellStyle name="60% - Accent2" xfId="51"/>
-    <cellStyle name="Accent3" xfId="52"/>
-    <cellStyle name="20% - Accent3" xfId="53"/>
-    <cellStyle name="Accent4" xfId="54"/>
-    <cellStyle name="20% - Accent4" xfId="55"/>
-    <cellStyle name="40% - Accent4" xfId="56"/>
-    <cellStyle name="Accent5" xfId="57"/>
-    <cellStyle name="40% - Accent5" xfId="58"/>
-    <cellStyle name="60% - Accent5" xfId="59"/>
-    <cellStyle name="Accent6" xfId="60"/>
-    <cellStyle name="40% - Accent6" xfId="61"/>
-    <cellStyle name="60% - Accent6" xfId="62"/>
+    <cellStyle name="40% - Accent1" xfId="48"/>
+    <cellStyle name="Check Cell" xfId="49"/>
+    <cellStyle name="Heading 2" xfId="50"/>
+    <cellStyle name="Note" xfId="51"/>
+    <cellStyle name="Hyperlink" xfId="52"/>
+    <cellStyle name="60% - Accent4" xfId="53"/>
+    <cellStyle name="Followed Hyperlink" xfId="54"/>
+    <cellStyle name="40% - Accent3" xfId="55"/>
+    <cellStyle name="Warning Text" xfId="56"/>
+    <cellStyle name="40% - Accent2" xfId="57"/>
+    <cellStyle name="Title" xfId="58"/>
+    <cellStyle name="CExplanatory Text" xfId="59"/>
+    <cellStyle name="Heading 1" xfId="60"/>
+    <cellStyle name="Heading 3" xfId="61"/>
+    <cellStyle name="Heading 4" xfId="62"/>
+    <cellStyle name="Input" xfId="63"/>
+    <cellStyle name="60% - Accent3" xfId="64"/>
+    <cellStyle name="Good" xfId="65"/>
+    <cellStyle name="Output" xfId="66"/>
+    <cellStyle name="20% - Accent1" xfId="67"/>
+    <cellStyle name="Calculation" xfId="68"/>
+    <cellStyle name="Linked Cell" xfId="69"/>
+    <cellStyle name="Total" xfId="70"/>
+    <cellStyle name="Bad" xfId="71"/>
+    <cellStyle name="Neutral" xfId="72"/>
+    <cellStyle name="Accent1" xfId="73"/>
+    <cellStyle name="20% - Accent5" xfId="74"/>
+    <cellStyle name="60% - Accent1" xfId="75"/>
+    <cellStyle name="Accent2" xfId="76"/>
+    <cellStyle name="20% - Accent2" xfId="77"/>
+    <cellStyle name="20% - Accent6" xfId="78"/>
+    <cellStyle name="60% - Accent2" xfId="79"/>
+    <cellStyle name="Accent3" xfId="80"/>
+    <cellStyle name="20% - Accent3" xfId="81"/>
+    <cellStyle name="Accent4" xfId="82"/>
+    <cellStyle name="20% - Accent4" xfId="83"/>
+    <cellStyle name="40% - Accent4" xfId="84"/>
+    <cellStyle name="Accent5" xfId="85"/>
+    <cellStyle name="40% - Accent5" xfId="86"/>
+    <cellStyle name="60% - Accent5" xfId="87"/>
+    <cellStyle name="Accent6" xfId="88"/>
+    <cellStyle name="40% - Accent6" xfId="89"/>
+    <cellStyle name="60% - Accent6" xfId="90"/>
   </cellStyles>
   <tableStyles count="0"/>
   <colors>
@@ -871,6 +926,718 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" b="0" u="none" baseline="0"/>
+              <a:t>EFcore30Benchmark</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>DapperLoad</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$B$2:$B$5</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LazyLoad</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$C$2:$C$5</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>EagerLoad</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$D$2:$D$5</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>StoredProcedure</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$E$2:$E$5</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>NativeQuery</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$F$2:$F$5</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>DapperLoad</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$G$2:$G$5</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="25730616"/>
+        <c:axId val="30248956"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="25730616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:delete val="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="30248956"/>
+        <c:crosses val="autoZero"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="30248956"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:delete val="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="25730616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr rot="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US" u="none" baseline="0"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext>
+      <c:pivotOptions>
+        <c14 xmlns="dropZoneFilter" val="1"/>
+        <c14 xmlns="dropZoneCategories" val="1"/>
+        <c14 xmlns="dropZoneData" val="1"/>
+        <c14 xmlns="dropZoneSeries" val="1"/>
+        <c14 xmlns="dropZonesVisible" val="1"/>
+      </c:pivotOptions>
+    </c:ext>
+  </c:extLst>
+  <c:date1904 val="1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" u="none" baseline="0"/>
+              <a:t>EFcore30Benchmark</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>NativeQuery</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$B$18:$B$21</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LazyLoad</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$C$18:$C$21</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>EagerLoad</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$D$18:$D$21</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>StoredProcedure</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$E$18:$E$21</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>NativeQuery</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$F$18:$F$21</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>DapperLoad</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>FirstRunElapsed</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mean</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Max</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Min</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EFcore30Benchmark!$G$18:$G$21</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="3805153"/>
+        <c:axId val="34246385"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="3805153"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:delete val="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="34246385"/>
+        <c:crosses val="autoZero"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="34246385"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:delete val="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="3805153"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr rot="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US" u="none" baseline="0"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext>
+      <c:pivotOptions>
+        <c14 xmlns="dropZoneFilter" val="1"/>
+        <c14 xmlns="dropZoneCategories" val="1"/>
+        <c14 xmlns="dropZoneData" val="1"/>
+        <c14 xmlns="dropZoneSeries" val="1"/>
+        <c14 xmlns="dropZonesVisible" val="1"/>
+      </c:pivotOptions>
+    </c:ext>
+  </c:extLst>
+  <c:date1904 val="1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>EFcore30Benchmark</a:t>
             </a:r>
@@ -928,7 +1695,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EFcore30Benchmark!$B$2:$B$5</c:f>
+              <c:f>EFcore30Benchmark!$B$34:$B$37</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -970,7 +1737,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EFcore30Benchmark!$C$2:$C$5</c:f>
+              <c:f>EFcore30Benchmark!$C$34:$C$37</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -1012,7 +1779,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EFcore30Benchmark!$D$2:$D$5</c:f>
+              <c:f>EFcore30Benchmark!$D$34:$D$37</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -1054,7 +1821,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EFcore30Benchmark!$E$2:$E$5</c:f>
+              <c:f>EFcore30Benchmark!$E$34:$E$37</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -1096,7 +1863,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EFcore30Benchmark!$F$2:$F$5</c:f>
+              <c:f>EFcore30Benchmark!$F$34:$F$37</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -1138,16 +1905,16 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EFcore30Benchmark!$G$2:$G$5</c:f>
+              <c:f>EFcore30Benchmark!$G$34:$G$37</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="14363903"/>
-        <c:axId val="62166264"/>
+        <c:axId val="39782011"/>
+        <c:axId val="22493786"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="14363903"/>
+        <c:axId val="39782011"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1157,13 +1924,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62166264"/>
+        <c:crossAx val="22493786"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62166264"/>
+        <c:axId val="22493786"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,7 +1945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="14363903"/>
+        <c:crossAx val="39782011"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -1235,6 +2002,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6515100" y="2743200"/>
+        <a:ext cx="12801600" cy="2400300"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6515100" y="5486400"/>
+        <a:ext cx="12801600" cy="2400300"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1562,7 +2389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1748,22 +2575,338 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" ht="13.5" customHeight="1"/>
-    <row r="18" ht="13.5" customHeight="1"/>
-    <row r="19" ht="13.5" customHeight="1"/>
-    <row r="20" ht="13.5" customHeight="1"/>
-    <row r="21" ht="13.5" customHeight="1"/>
-    <row r="22" ht="13.5" customHeight="1"/>
-    <row r="23" ht="13.5" customHeight="1"/>
-    <row r="31" ht="13.5" customHeight="1"/>
-    <row r="33" ht="13.5" customHeight="1"/>
-    <row r="34" ht="13.5" customHeight="1"/>
-    <row r="35" ht="13.5" customHeight="1"/>
-    <row r="36" ht="13.5" customHeight="1"/>
-    <row r="37" ht="13.5" customHeight="1"/>
-    <row r="38" ht="13.5" customHeight="1"/>
-    <row r="39" ht="13.5" customHeight="1"/>
-    <row r="47" ht="13.5" customHeight="1"/>
+    <row r="17" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>1550.6259</v>
+      </c>
+      <c r="C18">
+        <v>94.0622</v>
+      </c>
+      <c r="D18">
+        <v>2.1603</v>
+      </c>
+      <c r="E18">
+        <v>9.2278</v>
+      </c>
+      <c r="F18">
+        <v>2.2459</v>
+      </c>
+      <c r="G18">
+        <v>129.4131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>2.3505632231404956</v>
+      </c>
+      <c r="C19">
+        <v>2.0540368257261417</v>
+      </c>
+      <c r="D19">
+        <v>2.0507946652719675</v>
+      </c>
+      <c r="E19">
+        <v>2.084652593360997</v>
+      </c>
+      <c r="F19">
+        <v>1.933873899371071</v>
+      </c>
+      <c r="G19">
+        <v>1.3881008565310486</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>35.3295</v>
+      </c>
+      <c r="C20">
+        <v>7.9795</v>
+      </c>
+      <c r="D20">
+        <v>5.6878</v>
+      </c>
+      <c r="E20">
+        <v>6.9774</v>
+      </c>
+      <c r="F20">
+        <v>6.3369</v>
+      </c>
+      <c r="G20">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>1.4305</v>
+      </c>
+      <c r="C21">
+        <v>1.4803</v>
+      </c>
+      <c r="D21">
+        <v>1.4746</v>
+      </c>
+      <c r="E21">
+        <v>1.4591</v>
+      </c>
+      <c r="F21">
+        <v>1.4129</v>
+      </c>
+      <c r="G21">
+        <v>0.9937</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" ht="13.5" customHeight="1">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>467.0055</v>
+      </c>
+      <c r="C34">
+        <v>991.0041</v>
+      </c>
+      <c r="D34">
+        <v>3.0013</v>
+      </c>
+      <c r="E34">
+        <v>16.5533</v>
+      </c>
+      <c r="F34">
+        <v>9.4833</v>
+      </c>
+      <c r="G34">
+        <v>1.7503</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>1.641999147121536</v>
+      </c>
+      <c r="C35">
+        <v>2.267055475206613</v>
+      </c>
+      <c r="D35">
+        <v>2.0954279411764705</v>
+      </c>
+      <c r="E35">
+        <v>2.1498549896049908</v>
+      </c>
+      <c r="F35">
+        <v>2.038473618352451</v>
+      </c>
+      <c r="G35">
+        <v>1.3774759139784942</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>44.0002</v>
+      </c>
+      <c r="C36">
+        <v>32.1686</v>
+      </c>
+      <c r="D36">
+        <v>9.2735</v>
+      </c>
+      <c r="E36">
+        <v>5.324</v>
+      </c>
+      <c r="F36">
+        <v>6.8542</v>
+      </c>
+      <c r="G36">
+        <v>6.5028</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>0.9823</v>
+      </c>
+      <c r="C37">
+        <v>1.5368</v>
+      </c>
+      <c r="D37">
+        <v>1.5205</v>
+      </c>
+      <c r="E37">
+        <v>1.5575</v>
+      </c>
+      <c r="F37">
+        <v>1.4754</v>
+      </c>
+      <c r="G37">
+        <v>1.0186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" ht="13.5" customHeight="1">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="49" ht="13.5" customHeight="1"/>
     <row r="50" ht="13.5" customHeight="1"/>
     <row r="51" ht="13.5" customHeight="1"/>

</xml_diff>